<commit_message>
Xuất danh sách sản phẩm ra file Excel
</commit_message>
<xml_diff>
--- a/CongDoanCoreApp/wwwroot/uploaded/excels/ProductImportTemplate.xlsx
+++ b/CongDoanCoreApp/wwwroot/uploaded/excels/ProductImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CongDoan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xây dựng ứng dụng web với ASP.NET Core\CongDoanCoreApp\CongDoanCoreApp\wwwroot\uploaded\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Description</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Seo Description</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
   <si>
     <t>Hot Flag</t>
@@ -127,9 +124,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0">
-  <autoFilter ref="A1:K23"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J23" totalsRowShown="0">
+  <autoFilter ref="A1:J23"/>
+  <tableColumns count="10">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="4" name="Original Price"/>
@@ -138,7 +135,6 @@
     <tableColumn id="8" name="Content"/>
     <tableColumn id="9" name="Seo Keywords"/>
     <tableColumn id="10" name="Seo Description"/>
-    <tableColumn id="11" name="Status"/>
     <tableColumn id="12" name="Home Flag"/>
     <tableColumn id="13" name="Hot Flag"/>
   </tableColumns>
@@ -409,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,12 +421,11 @@
     <col min="6" max="6" width="19" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -456,21 +451,18 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>1021</v>
@@ -482,21 +474,18 @@
         <v>1021</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
       <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>